<commit_message>
Update the fixtures fils
</commit_message>
<xml_diff>
--- a/cypress/fixtures/delivery same day DoorToCounter.xlsx
+++ b/cypress/fixtures/delivery same day DoorToCounter.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\it\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\it\MylerzEnd2End\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2459,8 +2459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>